<commit_message>
Updated file to console based on cn1112
</commit_message>
<xml_diff>
--- a/console/Domain-Name-and-Website/域名诊断待翻译文档.xlsx
+++ b/console/Domain-Name-and-Website/域名诊断待翻译文档.xlsx
@@ -1,27 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/echo_shi/Desktop/京东云-1114/译文/console-cn1114（2）-译文-提交-1/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E3E14928-AEBA-2F4F-AA02-21652C6739AB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="460" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5085" yWindow="-23145" windowWidth="21840" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}"/>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
+    <t>Domain Name Health Diagnosis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comprehensive intellectualized domain name diagnosis to check the domain name health status at any time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Diagnosis Items</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -50,6 +55,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>This domain name can be used normally</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The domain name will expire in ...</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Update Time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -66,10 +79,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>The domain name resolution is normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Details</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Please enter correct domain name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Detection failed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -347,37 +368,13 @@
       </rPr>
       <t>检测失败</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This domain can be used normally</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The domain will expire in ...</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The domain resolution is normal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Please enter correct domain</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Domain Health Diagnosis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Comprehensive intellectualized domain diagnosis to check the domain health status at any time.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -767,182 +764,182 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="45" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.625" style="2" customWidth="1"/>
     <col min="3" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>